<commit_message>
Started adding more to info.
- Minor fixes and tweaks here and there.
</commit_message>
<xml_diff>
--- a/resources/data-imports/quests.xlsx
+++ b/resources/data-imports/quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>name</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Artifact Crafting Book</t>
+  </si>
+  <si>
+    <t>Artifact Crafting Masters Book</t>
   </si>
   <si>
     <t>Forge Master</t>
@@ -487,7 +490,7 @@
     <col min="4" max="4" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="12" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="32" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="36" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="19" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="16" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="13" bestFit="true" customWidth="true" style="0"/>
@@ -629,7 +632,7 @@
         <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -646,16 +649,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H6">
         <v>1000</v>
@@ -672,16 +675,16 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7">
         <v>1000</v>
@@ -698,16 +701,16 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H8">
         <v>1000</v>
@@ -724,16 +727,16 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H9">
         <v>1000</v>
@@ -750,16 +753,16 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H10">
         <v>2000</v>

</xml_diff>

<commit_message>
Started adding sepecial location docs.
- Refactored the way we handle quests.
- Fixed tests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/quests.xlsx
+++ b/resources/data-imports/quests.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC810A8A-79A7-5742-B8FA-4B82DB41AB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Quests" sheetId="1" r:id="rId4"/>
+    <sheet name="Quests" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="112">
   <si>
     <t>name</t>
   </si>
@@ -348,19 +364,17 @@
   </si>
   <si>
     <t>Bag of Chance</t>
+  </si>
+  <si>
+    <t>is_parent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -371,28 +385,37 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -682,38 +705,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:Q33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="34" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="36" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="43" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="34" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" customWidth="1"/>
+    <col min="15" max="15" width="43" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -754,19 +774,22 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>111</v>
+      </c>
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -794,8 +817,11 @@
       <c r="M2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -820,8 +846,11 @@
       <c r="K3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -846,8 +875,11 @@
       <c r="K4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -872,8 +904,11 @@
       <c r="K5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -898,8 +933,11 @@
       <c r="K6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -924,45 +962,54 @@
       <c r="K7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>63</v>
+      </c>
+      <c r="D8">
+        <v>50000</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="H8">
+        <v>100000</v>
+      </c>
+      <c r="I8">
         <v>1000</v>
       </c>
-      <c r="I8">
-        <v>5</v>
-      </c>
       <c r="J8">
-        <v>100000</v>
+        <v>2000000000</v>
       </c>
       <c r="K8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>100</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>5000</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H9">
         <v>1000</v>
@@ -971,104 +1018,122 @@
         <v>10</v>
       </c>
       <c r="J9">
-        <v>1000</v>
+        <v>2000000</v>
       </c>
       <c r="K9">
-        <v>10</v>
-      </c>
-      <c r="N9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>100</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>25000</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10">
-        <v>2000</v>
-      </c>
-      <c r="I10">
-        <v>15</v>
-      </c>
-      <c r="J10">
-        <v>5000</v>
-      </c>
-      <c r="K10">
-        <v>20</v>
-      </c>
-      <c r="N10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>49</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>5000</v>
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H11">
         <v>1000</v>
       </c>
       <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>100000</v>
+      </c>
+      <c r="K11">
         <v>10</v>
       </c>
-      <c r="J11">
-        <v>2000000</v>
-      </c>
-      <c r="K11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12">
-        <v>25000</v>
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>43</v>
+      </c>
+      <c r="H12">
+        <v>1000</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>1000</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="O12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13">
+        <v>2000</v>
+      </c>
+      <c r="I13">
+        <v>15</v>
+      </c>
+      <c r="J13">
+        <v>5000</v>
+      </c>
+      <c r="K13">
+        <v>20</v>
+      </c>
+      <c r="O13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13">
-        <v>25000</v>
-      </c>
-      <c r="G13" t="s">
-        <v>51</v>
-      </c>
-      <c r="N13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" t="s">
-        <v>52</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -1077,102 +1142,90 @@
         <v>25000</v>
       </c>
       <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="O14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>25000</v>
+      </c>
+      <c r="G15" t="s">
         <v>53</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
-      <c r="A15" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15">
-        <v>30000</v>
-      </c>
-      <c r="G15" t="s">
-        <v>56</v>
-      </c>
-      <c r="N15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" t="s">
-        <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>55</v>
       </c>
       <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16">
+        <v>30000</v>
+      </c>
+      <c r="G16" t="s">
         <v>56</v>
       </c>
-      <c r="D16">
-        <v>50000</v>
-      </c>
-      <c r="G16" t="s">
-        <v>58</v>
-      </c>
-      <c r="N16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="O16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
         <v>55</v>
       </c>
       <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17">
+        <v>50000</v>
+      </c>
+      <c r="G17" t="s">
         <v>58</v>
       </c>
-      <c r="D17">
+      <c r="O17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18">
         <v>75000</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" t="s">
         <v>60</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18">
-        <v>50000</v>
-      </c>
-      <c r="G18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18">
-        <v>100000</v>
-      </c>
-      <c r="I18">
-        <v>1000</v>
-      </c>
-      <c r="J18">
-        <v>2000000000</v>
-      </c>
-      <c r="K18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1200,17 +1253,17 @@
       <c r="K19">
         <v>100</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>45</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>67</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -1241,17 +1294,17 @@
       <c r="K20">
         <v>100</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>65</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>72</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -1282,20 +1335,20 @@
       <c r="K21">
         <v>100</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>45</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>71</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>76</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -1326,20 +1379,20 @@
       <c r="K22">
         <v>100</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>73</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>81</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>82</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -1373,20 +1426,20 @@
       <c r="K23">
         <v>100</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>68</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>75</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>67</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -1408,11 +1461,11 @@
       <c r="K24">
         <v>50</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -1434,17 +1487,17 @@
       <c r="K25">
         <v>100</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>85</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>89</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -1475,14 +1528,14 @@
       <c r="K26">
         <v>75</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>83</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>93</v>
       </c>
@@ -1501,17 +1554,17 @@
       <c r="K27">
         <v>100</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>89</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -1536,14 +1589,14 @@
       <c r="K28">
         <v>85</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>87</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>98</v>
       </c>
@@ -1577,14 +1630,14 @@
       <c r="K29">
         <v>100</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>94</v>
       </c>
-      <c r="O29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="P29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -1606,11 +1659,11 @@
       <c r="K30">
         <v>100</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -1635,17 +1688,17 @@
       <c r="K31">
         <v>100</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>101</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>89</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>106</v>
       </c>
@@ -1670,11 +1723,11 @@
       <c r="K32">
         <v>100</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>109</v>
       </c>
@@ -1705,25 +1758,16 @@
       <c r="K33">
         <v>100</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>59</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>